<commit_message>
fix bug on calculate how many sequence get supplied data from pubmed
</commit_message>
<xml_diff>
--- a/OutputData/CCHF/Pubmed.xlsx
+++ b/OutputData/CCHF/Pubmed.xlsx
@@ -2460,7 +2460,7 @@
       <c r="O16" t="inlineStr"/>
       <c r="P16" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>sw13 cells</t>
         </is>
       </c>
       <c r="Q16" t="inlineStr"/>
@@ -2494,7 +2494,7 @@
       <c r="Y16" t="inlineStr"/>
       <c r="Z16" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>sw13 cells</t>
         </is>
       </c>
       <c r="AA16" t="inlineStr">
@@ -15836,7 +15836,7 @@
       </c>
       <c r="P120" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>cell culture</t>
         </is>
       </c>
       <c r="Q120" t="inlineStr"/>
@@ -15873,7 +15873,7 @@
       <c r="Y120" t="inlineStr"/>
       <c r="Z120" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>cell culture</t>
         </is>
       </c>
       <c r="AA120" t="inlineStr">
@@ -18147,7 +18147,7 @@
       </c>
       <c r="P138" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>lab strain</t>
         </is>
       </c>
       <c r="Q138" t="inlineStr"/>
@@ -18177,7 +18177,7 @@
       <c r="Y138" t="inlineStr"/>
       <c r="Z138" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>lab strain</t>
         </is>
       </c>
       <c r="AA138" t="inlineStr">
@@ -22257,7 +22257,7 @@
       <c r="O170" t="inlineStr"/>
       <c r="P170" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>vero cell</t>
         </is>
       </c>
       <c r="Q170" t="inlineStr"/>
@@ -22295,7 +22295,7 @@
       <c r="Y170" t="inlineStr"/>
       <c r="Z170" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>vero cell</t>
         </is>
       </c>
       <c r="AA170" t="inlineStr">
@@ -25843,7 +25843,7 @@
       </c>
       <c r="P198" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>human</t>
         </is>
       </c>
       <c r="Q198" t="inlineStr">
@@ -25882,7 +25882,7 @@
       <c r="Y198" t="inlineStr"/>
       <c r="Z198" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>human</t>
         </is>
       </c>
       <c r="AA198" t="inlineStr">
@@ -25946,7 +25946,7 @@
       </c>
       <c r="P199" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>human</t>
         </is>
       </c>
       <c r="Q199" t="inlineStr">
@@ -25984,7 +25984,7 @@
       <c r="Y199" t="inlineStr"/>
       <c r="Z199" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>human</t>
         </is>
       </c>
       <c r="AA199" t="inlineStr">
@@ -26048,7 +26048,7 @@
       </c>
       <c r="P200" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>human</t>
         </is>
       </c>
       <c r="Q200" t="inlineStr"/>
@@ -26082,7 +26082,7 @@
       <c r="Y200" t="inlineStr"/>
       <c r="Z200" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>human</t>
         </is>
       </c>
       <c r="AA200" t="inlineStr">
@@ -26146,7 +26146,7 @@
       </c>
       <c r="P201" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>human</t>
         </is>
       </c>
       <c r="Q201" t="inlineStr"/>
@@ -26184,7 +26184,7 @@
       <c r="Y201" t="inlineStr"/>
       <c r="Z201" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>human</t>
         </is>
       </c>
       <c r="AA201" t="inlineStr">
@@ -26248,7 +26248,7 @@
       </c>
       <c r="P202" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>human</t>
         </is>
       </c>
       <c r="Q202" t="inlineStr"/>
@@ -26282,7 +26282,7 @@
       <c r="Y202" t="inlineStr"/>
       <c r="Z202" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>human</t>
         </is>
       </c>
       <c r="AA202" t="inlineStr">
@@ -26346,7 +26346,7 @@
       </c>
       <c r="P203" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>human</t>
         </is>
       </c>
       <c r="Q203" t="inlineStr">
@@ -26384,7 +26384,7 @@
       <c r="Y203" t="inlineStr"/>
       <c r="Z203" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>human</t>
         </is>
       </c>
       <c r="AA203" t="inlineStr">
@@ -26448,7 +26448,7 @@
       </c>
       <c r="P204" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>human</t>
         </is>
       </c>
       <c r="Q204" t="inlineStr">
@@ -26486,7 +26486,7 @@
       <c r="Y204" t="inlineStr"/>
       <c r="Z204" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>human</t>
         </is>
       </c>
       <c r="AA204" t="inlineStr">
@@ -26550,7 +26550,7 @@
       </c>
       <c r="P205" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>human</t>
         </is>
       </c>
       <c r="Q205" t="inlineStr">
@@ -26584,7 +26584,7 @@
       <c r="Y205" t="inlineStr"/>
       <c r="Z205" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>human</t>
         </is>
       </c>
       <c r="AA205" t="inlineStr">
@@ -26648,7 +26648,7 @@
       </c>
       <c r="P206" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>human</t>
         </is>
       </c>
       <c r="Q206" t="inlineStr">
@@ -26686,7 +26686,7 @@
       <c r="Y206" t="inlineStr"/>
       <c r="Z206" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>human</t>
         </is>
       </c>
       <c r="AA206" t="inlineStr">
@@ -27154,7 +27154,7 @@
       </c>
       <c r="P211" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>human</t>
         </is>
       </c>
       <c r="Q211" t="inlineStr">
@@ -27190,7 +27190,7 @@
       <c r="Y211" t="inlineStr"/>
       <c r="Z211" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>human</t>
         </is>
       </c>
       <c r="AA211" t="inlineStr">
@@ -27352,7 +27352,7 @@
       </c>
       <c r="P213" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>human</t>
         </is>
       </c>
       <c r="Q213" t="inlineStr">
@@ -27386,7 +27386,7 @@
       <c r="Y213" t="inlineStr"/>
       <c r="Z213" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>human</t>
         </is>
       </c>
       <c r="AA213" t="inlineStr">

</xml_diff>

<commit_message>
fix bugs, update isolate column comment if the isolate is not a clinical isolate.
</commit_message>
<xml_diff>
--- a/OutputData/CCHF/Pubmed.xlsx
+++ b/OutputData/CCHF/Pubmed.xlsx
@@ -711,7 +711,7 @@
       </c>
       <c r="AB2" t="inlineStr">
         <is>
-          <t>brain</t>
+          <t>Brain</t>
         </is>
       </c>
       <c r="AC2" t="n">
@@ -831,7 +831,7 @@
       </c>
       <c r="AB3" t="inlineStr">
         <is>
-          <t>blood</t>
+          <t>Blood</t>
         </is>
       </c>
       <c r="AC3" t="n">
@@ -1087,7 +1087,7 @@
       </c>
       <c r="AB5" t="inlineStr">
         <is>
-          <t>blood</t>
+          <t>Blood</t>
         </is>
       </c>
       <c r="AC5" t="n">
@@ -1348,7 +1348,7 @@
       </c>
       <c r="AB7" t="inlineStr">
         <is>
-          <t>blood</t>
+          <t>Blood</t>
         </is>
       </c>
       <c r="AC7" t="n">
@@ -1732,7 +1732,7 @@
       </c>
       <c r="AB10" t="inlineStr">
         <is>
-          <t>blood</t>
+          <t>Blood</t>
         </is>
       </c>
       <c r="AC10" t="n">
@@ -1864,7 +1864,7 @@
       </c>
       <c r="AB11" t="inlineStr">
         <is>
-          <t>blood</t>
+          <t>Blood</t>
         </is>
       </c>
       <c r="AC11" t="n">
@@ -1996,7 +1996,7 @@
       </c>
       <c r="AB12" t="inlineStr">
         <is>
-          <t>blood</t>
+          <t>Blood</t>
         </is>
       </c>
       <c r="AC12" t="n">
@@ -2128,7 +2128,7 @@
       </c>
       <c r="AB13" t="inlineStr">
         <is>
-          <t>blood</t>
+          <t>Blood</t>
         </is>
       </c>
       <c r="AC13" t="n">
@@ -2762,7 +2762,7 @@
       </c>
       <c r="AB18" t="inlineStr">
         <is>
-          <t>blood</t>
+          <t>Blood</t>
         </is>
       </c>
       <c r="AC18" t="n">
@@ -2898,7 +2898,7 @@
       </c>
       <c r="AB19" t="inlineStr">
         <is>
-          <t>blood</t>
+          <t>Blood</t>
         </is>
       </c>
       <c r="AC19" t="n">
@@ -3031,7 +3031,7 @@
       </c>
       <c r="AB20" t="inlineStr">
         <is>
-          <t>blood</t>
+          <t>Blood</t>
         </is>
       </c>
       <c r="AC20" t="n">
@@ -3166,7 +3166,7 @@
       </c>
       <c r="AB21" t="inlineStr">
         <is>
-          <t>blood</t>
+          <t>Blood</t>
         </is>
       </c>
       <c r="AC21" t="n">
@@ -3290,7 +3290,7 @@
       </c>
       <c r="AB22" t="inlineStr">
         <is>
-          <t>blood</t>
+          <t>Blood</t>
         </is>
       </c>
       <c r="AC22" t="n">
@@ -3414,7 +3414,7 @@
       </c>
       <c r="AB23" t="inlineStr">
         <is>
-          <t>blood</t>
+          <t>Blood</t>
         </is>
       </c>
       <c r="AC23" t="n">
@@ -3554,7 +3554,7 @@
       </c>
       <c r="AB24" t="inlineStr">
         <is>
-          <t>blood</t>
+          <t>Blood</t>
         </is>
       </c>
       <c r="AC24" t="n">
@@ -3922,7 +3922,7 @@
       </c>
       <c r="AB27" t="inlineStr">
         <is>
-          <t>blood</t>
+          <t>Blood</t>
         </is>
       </c>
       <c r="AC27" t="n">
@@ -4176,7 +4176,7 @@
       </c>
       <c r="AB29" t="inlineStr">
         <is>
-          <t>blood</t>
+          <t>Blood</t>
         </is>
       </c>
       <c r="AC29" t="n">
@@ -4308,7 +4308,7 @@
       </c>
       <c r="AB30" t="inlineStr">
         <is>
-          <t>brain</t>
+          <t>Brain</t>
         </is>
       </c>
       <c r="AC30" t="n">
@@ -4561,7 +4561,7 @@
       </c>
       <c r="AB32" t="inlineStr">
         <is>
-          <t>blood</t>
+          <t>Blood</t>
         </is>
       </c>
       <c r="AC32" t="n">
@@ -4693,7 +4693,7 @@
       </c>
       <c r="AB33" t="inlineStr">
         <is>
-          <t>blood and spleen</t>
+          <t>Blood and spleen</t>
         </is>
       </c>
       <c r="AC33" t="n">
@@ -4957,7 +4957,7 @@
       </c>
       <c r="AB35" t="inlineStr">
         <is>
-          <t>brain</t>
+          <t>Brain</t>
         </is>
       </c>
       <c r="AC35" t="n">
@@ -5221,7 +5221,7 @@
       </c>
       <c r="AB37" t="inlineStr">
         <is>
-          <t>blood</t>
+          <t>Blood</t>
         </is>
       </c>
       <c r="AC37" t="n">
@@ -5349,7 +5349,7 @@
       </c>
       <c r="AB38" t="inlineStr">
         <is>
-          <t>blood</t>
+          <t>Blood</t>
         </is>
       </c>
       <c r="AC38" t="n">
@@ -5485,7 +5485,7 @@
       </c>
       <c r="AB39" t="inlineStr">
         <is>
-          <t>blood</t>
+          <t>Blood</t>
         </is>
       </c>
       <c r="AC39" t="n">
@@ -5749,7 +5749,7 @@
       </c>
       <c r="AB41" t="inlineStr">
         <is>
-          <t>blood</t>
+          <t>Blood</t>
         </is>
       </c>
       <c r="AC41" t="n">
@@ -5881,7 +5881,7 @@
       </c>
       <c r="AB42" t="inlineStr">
         <is>
-          <t>blood</t>
+          <t>Blood</t>
         </is>
       </c>
       <c r="AC42" t="n">
@@ -6009,7 +6009,7 @@
       </c>
       <c r="AB43" t="inlineStr">
         <is>
-          <t>blood</t>
+          <t>Blood</t>
         </is>
       </c>
       <c r="AC43" t="n">
@@ -6134,7 +6134,7 @@
       </c>
       <c r="AB44" t="inlineStr">
         <is>
-          <t>blood</t>
+          <t>Blood</t>
         </is>
       </c>
       <c r="AC44" t="n">
@@ -6270,7 +6270,7 @@
       </c>
       <c r="AB45" t="inlineStr">
         <is>
-          <t>blood</t>
+          <t>Blood</t>
         </is>
       </c>
       <c r="AC45" t="n">
@@ -6394,7 +6394,7 @@
       </c>
       <c r="AB46" t="inlineStr">
         <is>
-          <t>blood</t>
+          <t>Blood</t>
         </is>
       </c>
       <c r="AC46" t="n">
@@ -6526,7 +6526,7 @@
       </c>
       <c r="AB47" t="inlineStr">
         <is>
-          <t>blood</t>
+          <t>Blood</t>
         </is>
       </c>
       <c r="AC47" t="n">
@@ -6782,7 +6782,7 @@
       </c>
       <c r="AB49" t="inlineStr">
         <is>
-          <t>blood</t>
+          <t>Blood</t>
         </is>
       </c>
       <c r="AC49" t="n">
@@ -7042,7 +7042,7 @@
       </c>
       <c r="AB51" t="inlineStr">
         <is>
-          <t>blood</t>
+          <t>Blood</t>
         </is>
       </c>
       <c r="AC51" t="n">
@@ -7278,7 +7278,7 @@
       </c>
       <c r="AB53" t="inlineStr">
         <is>
-          <t>blood</t>
+          <t>Blood</t>
         </is>
       </c>
       <c r="AC53" t="n">
@@ -7527,7 +7527,7 @@
       </c>
       <c r="AB55" t="inlineStr">
         <is>
-          <t>blood</t>
+          <t>Blood</t>
         </is>
       </c>
       <c r="AC55" t="n">
@@ -7651,7 +7651,7 @@
       </c>
       <c r="AB56" t="inlineStr">
         <is>
-          <t>blood</t>
+          <t>Blood</t>
         </is>
       </c>
       <c r="AC56" t="n">
@@ -7908,7 +7908,7 @@
       </c>
       <c r="AB58" t="inlineStr">
         <is>
-          <t>blood</t>
+          <t>Blood</t>
         </is>
       </c>
       <c r="AC58" t="n">
@@ -8160,7 +8160,7 @@
       </c>
       <c r="AB60" t="inlineStr">
         <is>
-          <t>blood</t>
+          <t>Blood</t>
         </is>
       </c>
       <c r="AC60" t="n">
@@ -8536,7 +8536,7 @@
       </c>
       <c r="AB63" t="inlineStr">
         <is>
-          <t>blood</t>
+          <t>Blood</t>
         </is>
       </c>
       <c r="AC63" t="n">
@@ -8660,7 +8660,7 @@
       </c>
       <c r="AB64" t="inlineStr">
         <is>
-          <t>blood</t>
+          <t>Blood</t>
         </is>
       </c>
       <c r="AC64" t="inlineStr"/>
@@ -8786,7 +8786,7 @@
       </c>
       <c r="AB65" t="inlineStr">
         <is>
-          <t>blood</t>
+          <t>Blood</t>
         </is>
       </c>
       <c r="AC65" t="n">
@@ -9044,7 +9044,7 @@
       </c>
       <c r="AB67" t="inlineStr">
         <is>
-          <t>blood</t>
+          <t>Blood</t>
         </is>
       </c>
       <c r="AC67" t="n">
@@ -9176,7 +9176,7 @@
       </c>
       <c r="AB68" t="inlineStr">
         <is>
-          <t>blood</t>
+          <t>Blood</t>
         </is>
       </c>
       <c r="AC68" t="n">
@@ -9304,7 +9304,7 @@
       </c>
       <c r="AB69" t="inlineStr">
         <is>
-          <t>blood</t>
+          <t>Blood</t>
         </is>
       </c>
       <c r="AC69" t="n">
@@ -9566,7 +9566,7 @@
       </c>
       <c r="AB71" t="inlineStr">
         <is>
-          <t>blood</t>
+          <t>Blood</t>
         </is>
       </c>
       <c r="AC71" t="n">
@@ -9694,7 +9694,7 @@
       </c>
       <c r="AB72" t="inlineStr">
         <is>
-          <t>blood</t>
+          <t>Blood</t>
         </is>
       </c>
       <c r="AC72" t="n">
@@ -9824,7 +9824,7 @@
       </c>
       <c r="AB73" t="inlineStr">
         <is>
-          <t>blood</t>
+          <t>Blood</t>
         </is>
       </c>
       <c r="AC73" t="n">
@@ -9952,7 +9952,7 @@
       </c>
       <c r="AB74" t="inlineStr">
         <is>
-          <t>blood</t>
+          <t>Blood</t>
         </is>
       </c>
       <c r="AC74" t="n">
@@ -10084,7 +10084,7 @@
       </c>
       <c r="AB75" t="inlineStr">
         <is>
-          <t>blood</t>
+          <t>Blood</t>
         </is>
       </c>
       <c r="AC75" t="n">
@@ -10721,7 +10721,7 @@
       </c>
       <c r="AB80" t="inlineStr">
         <is>
-          <t>blood</t>
+          <t>Blood</t>
         </is>
       </c>
       <c r="AC80" t="n">
@@ -11118,7 +11118,7 @@
       </c>
       <c r="AB83" t="inlineStr">
         <is>
-          <t>brain</t>
+          <t>Brain</t>
         </is>
       </c>
       <c r="AC83" t="n">
@@ -11506,7 +11506,7 @@
       </c>
       <c r="AB86" t="inlineStr">
         <is>
-          <t>blood</t>
+          <t>Blood</t>
         </is>
       </c>
       <c r="AC86" t="n">
@@ -11882,7 +11882,7 @@
       </c>
       <c r="AB89" t="inlineStr">
         <is>
-          <t>blood</t>
+          <t>Blood</t>
         </is>
       </c>
       <c r="AC89" t="n">
@@ -12008,7 +12008,7 @@
       </c>
       <c r="AB90" t="inlineStr">
         <is>
-          <t>blood</t>
+          <t>Blood</t>
         </is>
       </c>
       <c r="AC90" t="n">
@@ -12271,7 +12271,7 @@
       </c>
       <c r="AB92" t="inlineStr">
         <is>
-          <t>blood</t>
+          <t>Blood</t>
         </is>
       </c>
       <c r="AC92" t="n">
@@ -12535,7 +12535,7 @@
       </c>
       <c r="AB94" t="inlineStr">
         <is>
-          <t>blood</t>
+          <t>Blood</t>
         </is>
       </c>
       <c r="AC94" t="n">
@@ -12920,7 +12920,7 @@
       </c>
       <c r="AB97" t="inlineStr">
         <is>
-          <t>spleen</t>
+          <t>Spleen</t>
         </is>
       </c>
       <c r="AC97" t="n">
@@ -13048,7 +13048,7 @@
       </c>
       <c r="AB98" t="inlineStr">
         <is>
-          <t>blood</t>
+          <t>Blood</t>
         </is>
       </c>
       <c r="AC98" t="n">
@@ -13180,7 +13180,7 @@
       </c>
       <c r="AB99" t="inlineStr">
         <is>
-          <t>blood</t>
+          <t>Blood</t>
         </is>
       </c>
       <c r="AC99" t="n">
@@ -13312,7 +13312,7 @@
       </c>
       <c r="AB100" t="inlineStr">
         <is>
-          <t>blood</t>
+          <t>Blood</t>
         </is>
       </c>
       <c r="AC100" t="n">
@@ -13820,7 +13820,7 @@
       </c>
       <c r="AB104" t="inlineStr">
         <is>
-          <t>blood and spleen</t>
+          <t>Blood and spleen</t>
         </is>
       </c>
       <c r="AC104" t="n">
@@ -13952,7 +13952,7 @@
       </c>
       <c r="AB105" t="inlineStr">
         <is>
-          <t>brain</t>
+          <t>Brain</t>
         </is>
       </c>
       <c r="AC105" t="n">
@@ -14080,7 +14080,7 @@
       </c>
       <c r="AB106" t="inlineStr">
         <is>
-          <t>blood</t>
+          <t>Blood</t>
         </is>
       </c>
       <c r="AC106" t="n">
@@ -14472,7 +14472,7 @@
       </c>
       <c r="AB109" t="inlineStr">
         <is>
-          <t>blood</t>
+          <t>Blood</t>
         </is>
       </c>
       <c r="AC109" t="n">
@@ -15506,7 +15506,7 @@
       </c>
       <c r="AB117" t="inlineStr">
         <is>
-          <t>blood</t>
+          <t>Blood</t>
         </is>
       </c>
       <c r="AC117" t="n">
@@ -15634,7 +15634,7 @@
       </c>
       <c r="AB118" t="inlineStr">
         <is>
-          <t>blood</t>
+          <t>Blood</t>
         </is>
       </c>
       <c r="AC118" t="inlineStr"/>
@@ -16001,7 +16001,7 @@
       </c>
       <c r="AB121" t="inlineStr">
         <is>
-          <t>blood</t>
+          <t>Blood</t>
         </is>
       </c>
       <c r="AC121" t="n">
@@ -16259,7 +16259,7 @@
       </c>
       <c r="AB123" t="inlineStr">
         <is>
-          <t>brain</t>
+          <t>Brain</t>
         </is>
       </c>
       <c r="AC123" t="n">
@@ -16651,7 +16651,7 @@
       </c>
       <c r="AB126" t="inlineStr">
         <is>
-          <t>blood</t>
+          <t>Blood</t>
         </is>
       </c>
       <c r="AC126" t="n">
@@ -16783,7 +16783,7 @@
       </c>
       <c r="AB127" t="inlineStr">
         <is>
-          <t>blood</t>
+          <t>Blood</t>
         </is>
       </c>
       <c r="AC127" t="n">
@@ -16911,7 +16911,7 @@
       </c>
       <c r="AB128" t="inlineStr">
         <is>
-          <t>blood</t>
+          <t>Blood</t>
         </is>
       </c>
       <c r="AC128" t="inlineStr"/>
@@ -17041,7 +17041,7 @@
       </c>
       <c r="AB129" t="inlineStr">
         <is>
-          <t>blood</t>
+          <t>Blood</t>
         </is>
       </c>
       <c r="AC129" t="n">
@@ -17299,7 +17299,7 @@
       </c>
       <c r="AB131" t="inlineStr">
         <is>
-          <t>blood</t>
+          <t>Blood</t>
         </is>
       </c>
       <c r="AC131" t="n">
@@ -17431,7 +17431,7 @@
       </c>
       <c r="AB132" t="inlineStr">
         <is>
-          <t>blood</t>
+          <t>Blood</t>
         </is>
       </c>
       <c r="AC132" t="n">
@@ -18067,7 +18067,7 @@
       </c>
       <c r="AB137" t="inlineStr">
         <is>
-          <t>blood</t>
+          <t>Blood</t>
         </is>
       </c>
       <c r="AC137" t="n">
@@ -18313,7 +18313,7 @@
       </c>
       <c r="AB139" t="inlineStr">
         <is>
-          <t>blood</t>
+          <t>Blood</t>
         </is>
       </c>
       <c r="AC139" t="n">
@@ -18445,7 +18445,7 @@
       </c>
       <c r="AB140" t="inlineStr">
         <is>
-          <t>blood</t>
+          <t>Blood</t>
         </is>
       </c>
       <c r="AC140" t="n">
@@ -18577,7 +18577,7 @@
       </c>
       <c r="AB141" t="inlineStr">
         <is>
-          <t>blood</t>
+          <t>Blood</t>
         </is>
       </c>
       <c r="AC141" t="n">
@@ -18705,7 +18705,7 @@
       </c>
       <c r="AB142" t="inlineStr">
         <is>
-          <t>blood</t>
+          <t>Blood</t>
         </is>
       </c>
       <c r="AC142" t="n">
@@ -19329,7 +19329,7 @@
       </c>
       <c r="AB147" t="inlineStr">
         <is>
-          <t>blood</t>
+          <t>Blood</t>
         </is>
       </c>
       <c r="AC147" t="n">
@@ -19463,7 +19463,7 @@
       </c>
       <c r="AB148" t="inlineStr">
         <is>
-          <t>nasal swab</t>
+          <t>Nasal swab</t>
         </is>
       </c>
       <c r="AC148" t="n">
@@ -19731,7 +19731,7 @@
       </c>
       <c r="AB150" t="inlineStr">
         <is>
-          <t>blood</t>
+          <t>Blood</t>
         </is>
       </c>
       <c r="AC150" t="n">
@@ -19991,7 +19991,7 @@
       </c>
       <c r="AB152" t="inlineStr">
         <is>
-          <t>blood</t>
+          <t>Blood</t>
         </is>
       </c>
       <c r="AC152" t="n">
@@ -20119,7 +20119,7 @@
       </c>
       <c r="AB153" t="inlineStr">
         <is>
-          <t>blood</t>
+          <t>Blood</t>
         </is>
       </c>
       <c r="AC153" t="n">
@@ -20513,7 +20513,7 @@
       </c>
       <c r="AB156" t="inlineStr">
         <is>
-          <t>blood</t>
+          <t>Blood</t>
         </is>
       </c>
       <c r="AC156" t="n">
@@ -21287,7 +21287,7 @@
       </c>
       <c r="AB162" t="inlineStr">
         <is>
-          <t>blood</t>
+          <t>Blood</t>
         </is>
       </c>
       <c r="AC162" t="n">
@@ -21537,7 +21537,7 @@
       </c>
       <c r="AB164" t="inlineStr">
         <is>
-          <t>blood</t>
+          <t>Blood</t>
         </is>
       </c>
       <c r="AC164" t="n">
@@ -22181,7 +22181,7 @@
       </c>
       <c r="AB169" t="inlineStr">
         <is>
-          <t>blood</t>
+          <t>Blood</t>
         </is>
       </c>
       <c r="AC169" t="n">
@@ -23182,7 +23182,7 @@
       </c>
       <c r="AB177" t="inlineStr">
         <is>
-          <t>blood</t>
+          <t>Blood</t>
         </is>
       </c>
       <c r="AC177" t="n">
@@ -23314,7 +23314,7 @@
       </c>
       <c r="AB178" t="inlineStr">
         <is>
-          <t>blood</t>
+          <t>Blood</t>
         </is>
       </c>
       <c r="AC178" t="n">
@@ -23954,7 +23954,7 @@
       </c>
       <c r="AB183" t="inlineStr">
         <is>
-          <t>blood</t>
+          <t>Blood</t>
         </is>
       </c>
       <c r="AC183" t="n">
@@ -24083,7 +24083,7 @@
       </c>
       <c r="AB184" t="inlineStr">
         <is>
-          <t>blood</t>
+          <t>Blood</t>
         </is>
       </c>
       <c r="AC184" t="n">
@@ -24211,7 +24211,7 @@
       </c>
       <c r="AB185" t="inlineStr">
         <is>
-          <t>blood</t>
+          <t>Blood</t>
         </is>
       </c>
       <c r="AC185" t="n">
@@ -24469,7 +24469,7 @@
       </c>
       <c r="AB187" t="inlineStr">
         <is>
-          <t>blood</t>
+          <t>Blood</t>
         </is>
       </c>
       <c r="AC187" t="n">
@@ -24867,7 +24867,7 @@
       </c>
       <c r="AB190" t="inlineStr">
         <is>
-          <t>blood</t>
+          <t>Blood</t>
         </is>
       </c>
       <c r="AC190" t="n">
@@ -24999,7 +24999,7 @@
       </c>
       <c r="AB191" t="inlineStr">
         <is>
-          <t>blood</t>
+          <t>Blood</t>
         </is>
       </c>
       <c r="AC191" t="n">
@@ -25397,7 +25397,7 @@
       </c>
       <c r="AB194" t="inlineStr">
         <is>
-          <t>blood</t>
+          <t>Blood</t>
         </is>
       </c>
       <c r="AC194" t="n">
@@ -25655,7 +25655,7 @@
       </c>
       <c r="AB196" t="inlineStr">
         <is>
-          <t>brain</t>
+          <t>Brain</t>
         </is>
       </c>
       <c r="AC196" t="n">
@@ -25787,7 +25787,7 @@
       </c>
       <c r="AB197" t="inlineStr">
         <is>
-          <t>blood</t>
+          <t>Blood</t>
         </is>
       </c>
       <c r="AC197" t="n">
@@ -25892,7 +25892,7 @@
       </c>
       <c r="AB198" t="inlineStr">
         <is>
-          <t>blood</t>
+          <t>Blood</t>
         </is>
       </c>
       <c r="AC198" t="inlineStr"/>
@@ -25994,7 +25994,7 @@
       </c>
       <c r="AB199" t="inlineStr">
         <is>
-          <t>blood</t>
+          <t>Blood</t>
         </is>
       </c>
       <c r="AC199" t="inlineStr"/>
@@ -26292,7 +26292,7 @@
       </c>
       <c r="AB202" t="inlineStr">
         <is>
-          <t>blood</t>
+          <t>Blood</t>
         </is>
       </c>
       <c r="AC202" t="inlineStr"/>
@@ -26394,7 +26394,7 @@
       </c>
       <c r="AB203" t="inlineStr">
         <is>
-          <t>blood</t>
+          <t>Blood</t>
         </is>
       </c>
       <c r="AC203" t="inlineStr"/>
@@ -26496,7 +26496,7 @@
       </c>
       <c r="AB204" t="inlineStr">
         <is>
-          <t>blood</t>
+          <t>Blood</t>
         </is>
       </c>
       <c r="AC204" t="inlineStr"/>
@@ -26696,7 +26696,7 @@
       </c>
       <c r="AB206" t="inlineStr">
         <is>
-          <t>blood</t>
+          <t>Blood</t>
         </is>
       </c>
       <c r="AC206" t="inlineStr"/>
@@ -26798,7 +26798,7 @@
       </c>
       <c r="AB207" t="inlineStr">
         <is>
-          <t>blood</t>
+          <t>Blood</t>
         </is>
       </c>
       <c r="AC207" t="inlineStr"/>
@@ -27200,7 +27200,7 @@
       </c>
       <c r="AB211" t="inlineStr">
         <is>
-          <t>blood</t>
+          <t>Blood</t>
         </is>
       </c>
       <c r="AC211" t="inlineStr"/>

</xml_diff>